<commit_message>
non working but logically correct white transition algorithm
</commit_message>
<xml_diff>
--- a/pesos.xlsx
+++ b/pesos.xlsx
@@ -104,15 +104,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -134,7 +134,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="20">
@@ -359,7 +358,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -646,11 +645,11 @@
   </sheetPr>
   <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B123" activeCellId="0" sqref="B123:G123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -794,19 +793,24 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="C4" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="D4" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="E4" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="F4" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="G4" s="9" t="n">
         <v>-1</v>
@@ -853,19 +857,24 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="C5" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="D5" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E5" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F5" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="G5" s="9" t="n">
         <v>-1</v>
@@ -912,19 +921,24 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="C6" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="D6" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E6" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="F6" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="G6" s="9" t="n">
         <v>-1</v>
@@ -971,19 +985,24 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C7" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="D7" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="E7" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="F7" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="G7" s="9" t="n">
         <v>-1</v>
@@ -1030,19 +1049,24 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="G8" s="9" t="n">
         <v>-1</v>
@@ -1112,19 +1136,24 @@
         <v>1</v>
       </c>
       <c r="B10" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="C10" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D10" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="E10" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="F10" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>-1</v>
@@ -1171,19 +1200,24 @@
         <v>2</v>
       </c>
       <c r="B11" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="C11" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="D11" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E11" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="F11" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="G11" s="9" t="n">
         <v>-1</v>
@@ -1230,19 +1264,24 @@
         <v>3</v>
       </c>
       <c r="B12" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="C12" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="D12" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="E12" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="F12" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="G12" s="9" t="n">
         <v>-1</v>
@@ -1289,19 +1328,24 @@
         <v>4</v>
       </c>
       <c r="B13" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="C13" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="D13" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="E13" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="F13" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="G13" s="9" t="n">
         <v>-1</v>
@@ -1348,19 +1392,24 @@
         <v>5</v>
       </c>
       <c r="B14" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="C14" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="D14" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="E14" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="F14" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="G14" s="9" t="n">
         <v>-1</v>
@@ -1430,19 +1479,24 @@
         <v>1</v>
       </c>
       <c r="B16" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="C16" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="D16" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="E16" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="F16" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="G16" s="9" t="n">
         <v>-1</v>
@@ -1489,19 +1543,24 @@
         <v>2</v>
       </c>
       <c r="B17" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="C17" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="D17" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="E17" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="F17" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="G17" s="9" t="n">
         <v>-1</v>
@@ -1548,19 +1607,24 @@
         <v>3</v>
       </c>
       <c r="B18" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="C18" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="D18" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="E18" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="F18" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="G18" s="9" t="n">
         <v>-1</v>
@@ -1607,19 +1671,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="C19" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D19" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="E19" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="F19" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>-1</v>
@@ -1666,19 +1735,24 @@
         <v>5</v>
       </c>
       <c r="B20" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="C20" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="D20" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E20" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="F20" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="G20" s="9" t="n">
         <v>-1</v>
@@ -1748,19 +1822,24 @@
         <v>1</v>
       </c>
       <c r="B22" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="C22" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="D22" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E22" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="F22" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="G22" s="9" t="n">
         <v>-1</v>
@@ -1807,19 +1886,24 @@
         <v>2</v>
       </c>
       <c r="B23" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
       <c r="C23" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
+      </c>
+      <c r="D23" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
-      <c r="D23" s="9" t="n">
-        <v>25</v>
-      </c>
       <c r="E23" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="F23" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="G23" s="9" t="n">
         <v>-1</v>
@@ -1866,19 +1950,24 @@
         <v>3</v>
       </c>
       <c r="B24" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="C24" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="D24" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E24" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="F24" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="G24" s="9" t="n">
         <v>-1</v>
@@ -1925,18 +2014,23 @@
         <v>4</v>
       </c>
       <c r="B25" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="C25" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D25" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="E25" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F25" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="G25" s="9" t="n">
@@ -1984,19 +2078,24 @@
         <v>5</v>
       </c>
       <c r="B26" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="C26" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="D26" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="E26" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="F26" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="G26" s="9" t="n">
         <v>-1</v>
@@ -2066,19 +2165,24 @@
         <v>1</v>
       </c>
       <c r="B28" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="C28" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D28" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E28" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="F28" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="G28" s="9" t="n">
         <v>-1</v>
@@ -2125,19 +2229,24 @@
         <v>2</v>
       </c>
       <c r="B29" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C29" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="D29" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="E29" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="F29" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="G29" s="9" t="n">
         <v>-1</v>
@@ -2184,19 +2293,24 @@
         <v>3</v>
       </c>
       <c r="B30" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="C30" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="D30" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="E30" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="F30" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="G30" s="9" t="n">
         <v>-1</v>
@@ -2243,19 +2357,24 @@
         <v>4</v>
       </c>
       <c r="B31" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="C31" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="D31" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="E31" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F31" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="G31" s="9" t="n">
         <v>-1</v>
@@ -2302,19 +2421,24 @@
         <v>5</v>
       </c>
       <c r="B32" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="C32" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="D32" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="E32" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="F32" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="G32" s="9" t="n">
         <v>-1</v>
@@ -2384,19 +2508,24 @@
         <v>1</v>
       </c>
       <c r="B34" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="C34" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="D34" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="E34" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="F34" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="G34" s="9" t="n">
         <v>-1</v>
@@ -2443,19 +2572,24 @@
         <v>2</v>
       </c>
       <c r="B35" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="C35" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D35" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="E35" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="F35" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="G35" s="9" t="n">
         <v>-1</v>
@@ -2502,19 +2636,24 @@
         <v>3</v>
       </c>
       <c r="B36" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="C36" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="D36" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="E36" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="F36" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="G36" s="9" t="n">
         <v>-1</v>
@@ -2561,19 +2700,24 @@
         <v>4</v>
       </c>
       <c r="B37" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="C37" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="D37" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="E37" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="F37" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G37" s="9" t="n">
         <v>-1</v>
@@ -2620,19 +2764,24 @@
         <v>5</v>
       </c>
       <c r="B38" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="C38" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="D38" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="E38" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="F38" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="G38" s="9" t="n">
         <v>-1</v>
@@ -2702,18 +2851,23 @@
         <v>1</v>
       </c>
       <c r="B40" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
       <c r="C40" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="D40" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="E40" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="F40" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="G40" s="9" t="n">
@@ -2761,19 +2915,24 @@
         <v>2</v>
       </c>
       <c r="B41" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="C41" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="D41" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="E41" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="F41" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G41" s="9" t="n">
         <v>-1</v>
@@ -2820,19 +2979,24 @@
         <v>3</v>
       </c>
       <c r="B42" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="C42" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="D42" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="E42" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F42" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="G42" s="9" t="n">
         <v>-1</v>
@@ -2879,19 +3043,24 @@
         <v>4</v>
       </c>
       <c r="B43" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="C43" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D43" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="E43" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F43" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="G43" s="9" t="n">
         <v>-1</v>
@@ -2938,19 +3107,24 @@
         <v>5</v>
       </c>
       <c r="B44" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C44" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="D44" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="E44" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="F44" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="G44" s="9" t="n">
         <v>-1</v>
@@ -3020,19 +3194,24 @@
         <v>1</v>
       </c>
       <c r="B46" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="C46" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="D46" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="E46" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="F46" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="G46" s="9" t="n">
         <v>-1</v>
@@ -3079,19 +3258,24 @@
         <v>2</v>
       </c>
       <c r="B47" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="C47" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="D47" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="E47" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="F47" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="G47" s="9" t="n">
         <v>-1</v>
@@ -3138,19 +3322,24 @@
         <v>3</v>
       </c>
       <c r="B48" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="C48" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="D48" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="E48" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="F48" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="G48" s="9" t="n">
         <v>-1</v>
@@ -3197,19 +3386,24 @@
         <v>4</v>
       </c>
       <c r="B49" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C49" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D49" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="E49" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F49" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="G49" s="9" t="n">
         <v>-1</v>
@@ -3256,19 +3450,24 @@
         <v>5</v>
       </c>
       <c r="B50" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
+      </c>
+      <c r="C50" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
+      </c>
+      <c r="D50" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
+      </c>
+      <c r="E50" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
-      <c r="C50" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="D50" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="E50" s="9" t="n">
-        <v>-1</v>
-      </c>
       <c r="F50" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="G50" s="9" t="n">
         <v>-1</v>
@@ -3338,19 +3537,24 @@
         <v>1</v>
       </c>
       <c r="B52" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="C52" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="D52" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E52" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="F52" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="G52" s="9" t="n">
         <v>-1</v>
@@ -3397,19 +3601,24 @@
         <v>2</v>
       </c>
       <c r="B53" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="C53" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="D53" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="E53" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="F53" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="G53" s="9" t="n">
         <v>-1</v>
@@ -3456,19 +3665,24 @@
         <v>3</v>
       </c>
       <c r="B54" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="C54" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="D54" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="E54" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="F54" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G54" s="9" t="n">
         <v>-1</v>
@@ -3515,19 +3729,24 @@
         <v>4</v>
       </c>
       <c r="B55" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="C55" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="D55" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="E55" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="F55" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="G55" s="9" t="n">
         <v>-1</v>
@@ -3574,19 +3793,24 @@
         <v>5</v>
       </c>
       <c r="B56" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="C56" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="D56" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="E56" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="F56" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="G56" s="9" t="n">
         <v>-1</v>
@@ -3656,19 +3880,24 @@
         <v>1</v>
       </c>
       <c r="B58" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="C58" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="D58" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E58" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="F58" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="G58" s="9" t="n">
         <v>-1</v>
@@ -3715,19 +3944,24 @@
         <v>2</v>
       </c>
       <c r="B59" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="C59" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D59" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E59" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="F59" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="G59" s="9" t="n">
         <v>-1</v>
@@ -3774,19 +4008,24 @@
         <v>3</v>
       </c>
       <c r="B60" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="C60" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="D60" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="E60" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="F60" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="G60" s="9" t="n">
         <v>-1</v>
@@ -3833,19 +4072,24 @@
         <v>4</v>
       </c>
       <c r="B61" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="C61" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D61" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="E61" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="F61" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="G61" s="9" t="n">
         <v>-1</v>
@@ -3892,19 +4136,24 @@
         <v>5</v>
       </c>
       <c r="B62" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="C62" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="D62" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="E62" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="F62" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G62" s="9" t="n">
         <v>-1</v>
@@ -3974,19 +4223,24 @@
         <v>1</v>
       </c>
       <c r="B64" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C64" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="D64" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="E64" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="F64" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="G64" s="9" t="n">
         <v>-1</v>
@@ -4033,19 +4287,24 @@
         <v>2</v>
       </c>
       <c r="B65" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="C65" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="D65" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E65" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="F65" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="G65" s="9" t="n">
         <v>-1</v>
@@ -4092,19 +4351,24 @@
         <v>3</v>
       </c>
       <c r="B66" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="C66" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="D66" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E66" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="F66" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="G66" s="9" t="n">
         <v>-1</v>
@@ -4151,19 +4415,24 @@
         <v>4</v>
       </c>
       <c r="B67" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="C67" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="D67" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="E67" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="F67" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="G67" s="9" t="n">
         <v>-1</v>
@@ -4210,19 +4479,24 @@
         <v>5</v>
       </c>
       <c r="B68" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
+      </c>
+      <c r="C68" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
+      </c>
+      <c r="D68" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
+      </c>
+      <c r="E68" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
+      </c>
+      <c r="F68" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
-      </c>
-      <c r="C68" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="D68" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="E68" s="9" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F68" s="9" t="n">
-        <v>-1</v>
       </c>
       <c r="G68" s="9" t="n">
         <v>-1</v>
@@ -4292,19 +4566,24 @@
         <v>1</v>
       </c>
       <c r="B70" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C70" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="D70" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="E70" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F70" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G70" s="9" t="n">
         <v>-1</v>
@@ -4351,19 +4630,24 @@
         <v>2</v>
       </c>
       <c r="B71" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C71" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="D71" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="E71" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="F71" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="G71" s="9" t="n">
         <v>-1</v>
@@ -4410,19 +4694,24 @@
         <v>3</v>
       </c>
       <c r="B72" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="C72" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="D72" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="E72" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="F72" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G72" s="9" t="n">
         <v>-1</v>
@@ -4469,19 +4758,24 @@
         <v>4</v>
       </c>
       <c r="B73" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="C73" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D73" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="E73" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="F73" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="G73" s="9" t="n">
         <v>-1</v>
@@ -4528,19 +4822,24 @@
         <v>5</v>
       </c>
       <c r="B74" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="C74" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="D74" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="E74" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="F74" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="G74" s="9" t="n">
         <v>-1</v>
@@ -4610,19 +4909,24 @@
         <v>1</v>
       </c>
       <c r="B76" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="C76" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D76" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="E76" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="F76" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="G76" s="9" t="n">
         <v>-1</v>
@@ -4669,19 +4973,24 @@
         <v>2</v>
       </c>
       <c r="B77" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="C77" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="D77" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="E77" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="F77" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="G77" s="9" t="n">
         <v>-1</v>
@@ -4728,19 +5037,24 @@
         <v>3</v>
       </c>
       <c r="B78" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
+      </c>
+      <c r="C78" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
+      </c>
+      <c r="D78" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
-      <c r="C78" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="D78" s="9" t="n">
-        <v>25</v>
-      </c>
       <c r="E78" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="F78" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="G78" s="9" t="n">
         <v>-1</v>
@@ -4787,19 +5101,24 @@
         <v>4</v>
       </c>
       <c r="B79" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="C79" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D79" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="E79" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="F79" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="G79" s="9" t="n">
         <v>-1</v>
@@ -4846,19 +5165,24 @@
         <v>5</v>
       </c>
       <c r="B80" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="C80" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="D80" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="E80" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="F80" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="G80" s="9" t="n">
         <v>-1</v>
@@ -4928,19 +5252,24 @@
         <v>1</v>
       </c>
       <c r="B82" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="C82" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="D82" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="E82" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="F82" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="G82" s="9" t="n">
         <v>-1</v>
@@ -4987,19 +5316,24 @@
         <v>2</v>
       </c>
       <c r="B83" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="C83" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="D83" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="E83" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="F83" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="G83" s="9" t="n">
         <v>-1</v>
@@ -5046,19 +5380,24 @@
         <v>3</v>
       </c>
       <c r="B84" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="C84" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="D84" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="E84" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="F84" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="G84" s="9" t="n">
         <v>-1</v>
@@ -5105,19 +5444,24 @@
         <v>4</v>
       </c>
       <c r="B85" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="C85" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="D85" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="E85" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="F85" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="G85" s="9" t="n">
         <v>-1</v>
@@ -5164,19 +5508,24 @@
         <v>5</v>
       </c>
       <c r="B86" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
+      </c>
+      <c r="C86" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
-      <c r="C86" s="9" t="n">
-        <v>25</v>
-      </c>
       <c r="D86" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="E86" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F86" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="G86" s="9" t="n">
         <v>-1</v>
@@ -5246,19 +5595,24 @@
         <v>1</v>
       </c>
       <c r="B88" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="C88" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="D88" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="E88" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="F88" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G88" s="9" t="n">
         <v>-1</v>
@@ -5305,19 +5659,24 @@
         <v>2</v>
       </c>
       <c r="B89" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
+      </c>
+      <c r="C89" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
+      </c>
+      <c r="D89" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
-      <c r="C89" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="D89" s="9" t="n">
-        <v>25</v>
-      </c>
       <c r="E89" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="F89" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="G89" s="9" t="n">
         <v>-1</v>
@@ -5364,19 +5723,24 @@
         <v>3</v>
       </c>
       <c r="B90" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C90" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="D90" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="E90" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="F90" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="G90" s="9" t="n">
         <v>-1</v>
@@ -5423,19 +5787,24 @@
         <v>4</v>
       </c>
       <c r="B91" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C91" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="D91" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="E91" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F91" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="G91" s="9" t="n">
         <v>-1</v>
@@ -5482,19 +5851,24 @@
         <v>5</v>
       </c>
       <c r="B92" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="C92" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D92" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="E92" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="F92" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="G92" s="9" t="n">
         <v>-1</v>
@@ -5564,19 +5938,24 @@
         <v>1</v>
       </c>
       <c r="B94" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="C94" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="D94" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E94" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="F94" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G94" s="9" t="n">
         <v>-1</v>
@@ -5623,19 +6002,24 @@
         <v>2</v>
       </c>
       <c r="B95" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="C95" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="D95" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="E95" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="F95" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="G95" s="9" t="n">
         <v>-1</v>
@@ -5682,19 +6066,24 @@
         <v>3</v>
       </c>
       <c r="B96" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="C96" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="D96" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="E96" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="F96" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="G96" s="9" t="n">
         <v>-1</v>
@@ -5741,19 +6130,24 @@
         <v>4</v>
       </c>
       <c r="B97" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="C97" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="D97" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="E97" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="F97" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="G97" s="9" t="n">
         <v>-1</v>
@@ -5800,19 +6194,24 @@
         <v>5</v>
       </c>
       <c r="B98" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="C98" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="D98" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="E98" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="F98" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="G98" s="9" t="n">
         <v>-1</v>
@@ -5882,19 +6281,24 @@
         <v>1</v>
       </c>
       <c r="B100" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="C100" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="D100" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="E100" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="F100" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="G100" s="9" t="n">
         <v>-1</v>
@@ -5941,19 +6345,24 @@
         <v>2</v>
       </c>
       <c r="B101" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
+      </c>
+      <c r="C101" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
-      <c r="C101" s="9" t="n">
-        <v>25</v>
-      </c>
       <c r="D101" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E101" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="F101" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="G101" s="9" t="n">
         <v>-1</v>
@@ -6000,19 +6409,24 @@
         <v>3</v>
       </c>
       <c r="B102" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
       <c r="C102" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="D102" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E102" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="F102" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="G102" s="9" t="n">
         <v>-1</v>
@@ -6059,19 +6473,24 @@
         <v>4</v>
       </c>
       <c r="B103" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C103" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="D103" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="E103" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="F103" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="G103" s="9" t="n">
         <v>-1</v>
@@ -6118,19 +6537,24 @@
         <v>5</v>
       </c>
       <c r="B104" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="C104" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="D104" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="E104" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="F104" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="G104" s="9" t="n">
         <v>-1</v>
@@ -6200,19 +6624,24 @@
         <v>1</v>
       </c>
       <c r="B106" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="C106" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="D106" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E106" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F106" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="G106" s="9" t="n">
         <v>-1</v>
@@ -6259,19 +6688,24 @@
         <v>2</v>
       </c>
       <c r="B107" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="C107" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="D107" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="E107" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F107" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G107" s="9" t="n">
         <v>-1</v>
@@ -6318,19 +6752,24 @@
         <v>3</v>
       </c>
       <c r="B108" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="C108" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="D108" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="E108" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="F108" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="G108" s="9" t="n">
         <v>-1</v>
@@ -6377,19 +6816,24 @@
         <v>4</v>
       </c>
       <c r="B109" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
+      </c>
+      <c r="C109" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>25</v>
       </c>
-      <c r="C109" s="9" t="n">
-        <v>25</v>
-      </c>
       <c r="D109" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="E109" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="F109" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="G109" s="9" t="n">
         <v>-1</v>
@@ -6436,19 +6880,24 @@
         <v>5</v>
       </c>
       <c r="B110" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="C110" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="D110" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="E110" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F110" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="G110" s="9" t="n">
         <v>-1</v>
@@ -6518,19 +6967,24 @@
         <v>1</v>
       </c>
       <c r="B112" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="C112" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="D112" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="E112" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="F112" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="G112" s="9" t="n">
         <v>-1</v>
@@ -6577,19 +7031,24 @@
         <v>2</v>
       </c>
       <c r="B113" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="C113" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="D113" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="E113" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="F113" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="G113" s="9" t="n">
         <v>-1</v>
@@ -6636,19 +7095,24 @@
         <v>3</v>
       </c>
       <c r="B114" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="C114" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="D114" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="E114" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="F114" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="G114" s="9" t="n">
         <v>-1</v>
@@ -6695,19 +7159,24 @@
         <v>4</v>
       </c>
       <c r="B115" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C115" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="D115" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E115" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F115" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="G115" s="9" t="n">
         <v>-1</v>
@@ -6754,19 +7223,24 @@
         <v>5</v>
       </c>
       <c r="B116" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="C116" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="D116" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="E116" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="F116" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="G116" s="9" t="n">
         <v>-1</v>
@@ -6836,19 +7310,24 @@
         <v>1</v>
       </c>
       <c r="B118" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="C118" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="D118" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="E118" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="F118" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="G118" s="9" t="n">
         <v>-1</v>
@@ -6895,19 +7374,24 @@
         <v>2</v>
       </c>
       <c r="B119" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="C119" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="D119" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="E119" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="F119" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="G119" s="9" t="n">
         <v>-1</v>
@@ -6954,19 +7438,24 @@
         <v>3</v>
       </c>
       <c r="B120" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="C120" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="D120" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="E120" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="F120" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="G120" s="9" t="n">
         <v>-1</v>
@@ -7013,19 +7502,24 @@
         <v>4</v>
       </c>
       <c r="B121" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="C121" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="D121" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="E121" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="F121" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="G121" s="9" t="n">
         <v>-1</v>
@@ -7072,19 +7566,24 @@
         <v>5</v>
       </c>
       <c r="B122" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="C122" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D122" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="E122" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="F122" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="G122" s="9" t="n">
         <v>-1</v>
@@ -7154,18 +7653,23 @@
         <v>1</v>
       </c>
       <c r="B124" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="C124" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="D124" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="E124" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="F124" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="G124" s="9" t="n">
@@ -7213,18 +7717,23 @@
         <v>2</v>
       </c>
       <c r="B125" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="C125" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="D125" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="E125" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="F125" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="G125" s="9" t="n">
@@ -7272,19 +7781,24 @@
         <v>3</v>
       </c>
       <c r="B126" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="C126" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="D126" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="E126" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="F126" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="G126" s="9" t="n">
         <v>-1</v>
@@ -7331,19 +7845,24 @@
         <v>4</v>
       </c>
       <c r="B127" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="C127" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="D127" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="E127" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="F127" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="G127" s="9" t="n">
         <v>-1</v>
@@ -7390,19 +7909,24 @@
         <v>5</v>
       </c>
       <c r="B128" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="C128" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="D128" s="9" t="n">
-        <v>25</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E128" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="F128" s="9" t="n">
-        <v>-1</v>
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G128" s="9" t="n">
         <v>-1</v>

</xml_diff>

<commit_message>
working? white transition algorithm
</commit_message>
<xml_diff>
--- a/pesos.xlsx
+++ b/pesos.xlsx
@@ -645,8 +645,8 @@
   </sheetPr>
   <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B123" activeCellId="0" sqref="B123:G123"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1137,23 +1137,23 @@
       </c>
       <c r="B10" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-8</v>
+        <v>19</v>
       </c>
       <c r="C10" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="n">
+        <f aca="false">RANDBETWEEN(-10,25)</f>
         <v>11</v>
-      </c>
-      <c r="D10" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
-      </c>
-      <c r="E10" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
-      </c>
-      <c r="F10" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>-1</v>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B11" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="D11" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="F11" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G11" s="9" t="n">
         <v>-1</v>
@@ -1265,23 +1265,23 @@
       </c>
       <c r="B12" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <v>25</v>
       </c>
       <c r="D12" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E12" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="F12" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G12" s="9" t="n">
         <v>-1</v>
@@ -1329,23 +1329,23 @@
       </c>
       <c r="B13" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <v>-8</v>
       </c>
       <c r="C13" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <v>14</v>
       </c>
       <c r="D13" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="F13" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <v>-9</v>
       </c>
       <c r="G13" s="9" t="n">
         <v>-1</v>
@@ -1393,11 +1393,11 @@
       </c>
       <c r="B14" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="C14" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="D14" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
@@ -1405,11 +1405,11 @@
       </c>
       <c r="E14" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <v>-3</v>
       </c>
       <c r="F14" s="9" t="n">
         <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <v>21</v>
       </c>
       <c r="G14" s="9" t="n">
         <v>-1</v>

</xml_diff>

<commit_message>
fixed vacant transition TODO
</commit_message>
<xml_diff>
--- a/pesos.xlsx
+++ b/pesos.xlsx
@@ -113,6 +113,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -134,6 +135,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="20">
@@ -646,10 +648,10 @@
   <dimension ref="A1:S128"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -793,24 +795,24 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="C4" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="D4" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="E4" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="F4" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="G4" s="9" t="n">
         <v>-1</v>
@@ -849,7 +851,7 @@
         <v>-1</v>
       </c>
       <c r="S4" s="9" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,24 +859,24 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="C5" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-5</v>
       </c>
-      <c r="D5" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
-      </c>
-      <c r="E5" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
-      </c>
       <c r="F5" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="G5" s="9" t="n">
         <v>-1</v>
@@ -913,7 +915,7 @@
         <v>-1</v>
       </c>
       <c r="S5" s="9" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,24 +923,24 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="C6" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="D6" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="E6" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="F6" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="G6" s="9" t="n">
         <v>-1</v>
@@ -977,7 +979,7 @@
         <v>-1</v>
       </c>
       <c r="S6" s="9" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,24 +987,24 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="C7" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D7" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="E7" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="F7" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G7" s="9" t="n">
         <v>-1</v>
@@ -1041,7 +1043,7 @@
         <v>-1</v>
       </c>
       <c r="S7" s="9" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,24 +1051,24 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="C8" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="D8" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="E8" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="F8" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="G8" s="9" t="n">
         <v>-1</v>
@@ -1105,7 +1107,7 @@
         <v>-1</v>
       </c>
       <c r="S8" s="9" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1136,24 +1138,24 @@
         <v>1</v>
       </c>
       <c r="B10" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="C10" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D10" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="E10" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="F10" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>-1</v>
@@ -1200,24 +1202,24 @@
         <v>2</v>
       </c>
       <c r="B11" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="C11" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="D11" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="E11" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
+      </c>
+      <c r="F11" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>21</v>
-      </c>
-      <c r="F11" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
       </c>
       <c r="G11" s="9" t="n">
         <v>-1</v>
@@ -1264,24 +1266,24 @@
         <v>3</v>
       </c>
       <c r="B12" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="C12" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="D12" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="E12" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="F12" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="G12" s="9" t="n">
         <v>-1</v>
@@ -1328,24 +1330,24 @@
         <v>4</v>
       </c>
       <c r="B13" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
       </c>
       <c r="C13" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="D13" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="E13" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="F13" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="G13" s="9" t="n">
         <v>-1</v>
@@ -1392,24 +1394,24 @@
         <v>5</v>
       </c>
       <c r="B14" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="C14" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
+      </c>
+      <c r="D14" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-2</v>
       </c>
-      <c r="D14" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
-      </c>
       <c r="E14" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="F14" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="G14" s="9" t="n">
         <v>-1</v>
@@ -1479,24 +1481,24 @@
         <v>1</v>
       </c>
       <c r="B16" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="C16" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="D16" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="E16" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="F16" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="G16" s="9" t="n">
         <v>-1</v>
@@ -1543,24 +1545,24 @@
         <v>2</v>
       </c>
       <c r="B17" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="C17" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="D17" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="E17" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F17" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="G17" s="9" t="n">
         <v>-1</v>
@@ -1607,24 +1609,24 @@
         <v>3</v>
       </c>
       <c r="B18" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="C18" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D18" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E18" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
       </c>
       <c r="F18" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="G18" s="9" t="n">
         <v>-1</v>
@@ -1671,24 +1673,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
+      </c>
+      <c r="C19" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
+      </c>
+      <c r="D19" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
+      </c>
+      <c r="E19" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
+      </c>
+      <c r="F19" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>11</v>
-      </c>
-      <c r="C19" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
-      </c>
-      <c r="D19" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
-      </c>
-      <c r="E19" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
-      </c>
-      <c r="F19" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>0</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>-1</v>
@@ -1735,24 +1737,24 @@
         <v>5</v>
       </c>
       <c r="B20" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C20" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="D20" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E20" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="F20" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G20" s="9" t="n">
         <v>-1</v>
@@ -1822,24 +1824,24 @@
         <v>1</v>
       </c>
       <c r="B22" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="C22" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>20</v>
       </c>
       <c r="D22" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="E22" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="F22" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="G22" s="9" t="n">
         <v>-1</v>
@@ -1886,24 +1888,24 @@
         <v>2</v>
       </c>
       <c r="B23" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="C23" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="D23" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="E23" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>0</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="F23" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="G23" s="9" t="n">
         <v>-1</v>
@@ -1950,23 +1952,23 @@
         <v>3</v>
       </c>
       <c r="B24" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
       </c>
       <c r="C24" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="D24" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
       </c>
       <c r="E24" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="F24" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>1</v>
       </c>
       <c r="G24" s="9" t="n">
@@ -2014,24 +2016,24 @@
         <v>4</v>
       </c>
       <c r="B25" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="C25" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="D25" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E25" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="F25" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="G25" s="9" t="n">
         <v>-1</v>
@@ -2078,24 +2080,24 @@
         <v>5</v>
       </c>
       <c r="B26" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="C26" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="D26" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="E26" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="F26" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G26" s="9" t="n">
         <v>-1</v>
@@ -2165,24 +2167,24 @@
         <v>1</v>
       </c>
       <c r="B28" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="C28" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="D28" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="E28" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="F28" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="G28" s="9" t="n">
         <v>-1</v>
@@ -2229,24 +2231,24 @@
         <v>2</v>
       </c>
       <c r="B29" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="C29" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="D29" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="E29" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="F29" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="G29" s="9" t="n">
         <v>-1</v>
@@ -2293,24 +2295,24 @@
         <v>3</v>
       </c>
       <c r="B30" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="C30" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="D30" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E30" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="F30" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="G30" s="9" t="n">
         <v>-1</v>
@@ -2357,24 +2359,24 @@
         <v>4</v>
       </c>
       <c r="B31" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="C31" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D31" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
+      </c>
+      <c r="E31" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>5</v>
       </c>
-      <c r="E31" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
-      </c>
       <c r="F31" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G31" s="9" t="n">
         <v>-1</v>
@@ -2421,24 +2423,24 @@
         <v>5</v>
       </c>
       <c r="B32" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="C32" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="D32" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>20</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="E32" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="F32" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="G32" s="9" t="n">
         <v>-1</v>
@@ -2508,24 +2510,24 @@
         <v>1</v>
       </c>
       <c r="B34" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="C34" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="D34" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="E34" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="F34" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="G34" s="9" t="n">
         <v>-1</v>
@@ -2572,24 +2574,24 @@
         <v>2</v>
       </c>
       <c r="B35" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="C35" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="D35" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>22</v>
       </c>
       <c r="E35" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F35" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>20</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="G35" s="9" t="n">
         <v>-1</v>
@@ -2636,24 +2638,24 @@
         <v>3</v>
       </c>
       <c r="B36" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C36" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="D36" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="E36" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="F36" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="G36" s="9" t="n">
         <v>-1</v>
@@ -2700,24 +2702,24 @@
         <v>4</v>
       </c>
       <c r="B37" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
       </c>
       <c r="C37" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
+      </c>
+      <c r="D37" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>6</v>
       </c>
-      <c r="D37" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
-      </c>
       <c r="E37" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="F37" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G37" s="9" t="n">
         <v>-1</v>
@@ -2764,23 +2766,23 @@
         <v>5</v>
       </c>
       <c r="B38" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="C38" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="D38" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="E38" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="F38" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-3</v>
       </c>
       <c r="G38" s="9" t="n">
@@ -2851,24 +2853,24 @@
         <v>1</v>
       </c>
       <c r="B40" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="C40" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D40" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="E40" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="F40" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="G40" s="9" t="n">
         <v>-1</v>
@@ -2915,24 +2917,24 @@
         <v>2</v>
       </c>
       <c r="B41" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C41" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="D41" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="E41" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F41" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="G41" s="9" t="n">
         <v>-1</v>
@@ -2979,24 +2981,24 @@
         <v>3</v>
       </c>
       <c r="B42" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="C42" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D42" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="E42" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="F42" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="G42" s="9" t="n">
         <v>-1</v>
@@ -3043,24 +3045,24 @@
         <v>4</v>
       </c>
       <c r="B43" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="C43" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="D43" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="E43" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="F43" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="G43" s="9" t="n">
         <v>-1</v>
@@ -3107,24 +3109,24 @@
         <v>5</v>
       </c>
       <c r="B44" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="C44" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
+      </c>
+      <c r="D44" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>13</v>
       </c>
-      <c r="D44" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
-      </c>
       <c r="E44" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="F44" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="G44" s="9" t="n">
         <v>-1</v>
@@ -3194,24 +3196,24 @@
         <v>1</v>
       </c>
       <c r="B46" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C46" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="D46" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="E46" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="F46" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="G46" s="9" t="n">
         <v>-1</v>
@@ -3258,24 +3260,24 @@
         <v>2</v>
       </c>
       <c r="B47" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="C47" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>0</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="D47" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="E47" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
       </c>
       <c r="F47" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="G47" s="9" t="n">
         <v>-1</v>
@@ -3322,24 +3324,24 @@
         <v>3</v>
       </c>
       <c r="B48" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="C48" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="D48" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
+      </c>
+      <c r="E48" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
+      </c>
+      <c r="F48" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-3</v>
-      </c>
-      <c r="E48" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
-      </c>
-      <c r="F48" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
       </c>
       <c r="G48" s="9" t="n">
         <v>-1</v>
@@ -3386,24 +3388,24 @@
         <v>4</v>
       </c>
       <c r="B49" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="C49" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="D49" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E49" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="F49" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
       </c>
       <c r="G49" s="9" t="n">
         <v>-1</v>
@@ -3450,24 +3452,24 @@
         <v>5</v>
       </c>
       <c r="B50" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="C50" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="D50" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="E50" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="F50" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="G50" s="9" t="n">
         <v>-1</v>
@@ -3537,24 +3539,24 @@
         <v>1</v>
       </c>
       <c r="B52" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="C52" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="D52" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="E52" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>0</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="F52" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="G52" s="9" t="n">
         <v>-1</v>
@@ -3601,24 +3603,24 @@
         <v>2</v>
       </c>
       <c r="B53" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>20</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="C53" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D53" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="E53" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="F53" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G53" s="9" t="n">
         <v>-1</v>
@@ -3665,24 +3667,24 @@
         <v>3</v>
       </c>
       <c r="B54" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="C54" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="D54" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
+      </c>
+      <c r="E54" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-8</v>
+      </c>
+      <c r="F54" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-9</v>
-      </c>
-      <c r="E54" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
-      </c>
-      <c r="F54" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
       </c>
       <c r="G54" s="9" t="n">
         <v>-1</v>
@@ -3729,24 +3731,24 @@
         <v>4</v>
       </c>
       <c r="B55" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="C55" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="D55" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
+      </c>
+      <c r="E55" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>11</v>
       </c>
-      <c r="E55" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
-      </c>
       <c r="F55" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="G55" s="9" t="n">
         <v>-1</v>
@@ -3793,24 +3795,24 @@
         <v>5</v>
       </c>
       <c r="B56" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C56" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>0</v>
+      </c>
+      <c r="D56" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>24</v>
       </c>
-      <c r="D56" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
-      </c>
       <c r="E56" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="F56" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>20</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="G56" s="9" t="n">
         <v>-1</v>
@@ -3880,24 +3882,24 @@
         <v>1</v>
       </c>
       <c r="B58" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="C58" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="D58" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E58" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F58" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="G58" s="9" t="n">
         <v>-1</v>
@@ -3944,24 +3946,24 @@
         <v>2</v>
       </c>
       <c r="B59" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="C59" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="D59" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E59" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="F59" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="G59" s="9" t="n">
         <v>-1</v>
@@ -4008,24 +4010,24 @@
         <v>3</v>
       </c>
       <c r="B60" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="C60" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="D60" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="E60" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="F60" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="G60" s="9" t="n">
         <v>-1</v>
@@ -4072,24 +4074,24 @@
         <v>4</v>
       </c>
       <c r="B61" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="C61" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
+      </c>
+      <c r="D61" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
+      </c>
+      <c r="E61" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
+      </c>
+      <c r="F61" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-6</v>
-      </c>
-      <c r="D61" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
-      </c>
-      <c r="E61" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
-      </c>
-      <c r="F61" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
       </c>
       <c r="G61" s="9" t="n">
         <v>-1</v>
@@ -4136,24 +4138,24 @@
         <v>5</v>
       </c>
       <c r="B62" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="C62" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="D62" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="E62" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="F62" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="G62" s="9" t="n">
         <v>-1</v>
@@ -4223,24 +4225,24 @@
         <v>1</v>
       </c>
       <c r="B64" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="C64" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="D64" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>11</v>
       </c>
       <c r="E64" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="F64" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="G64" s="9" t="n">
         <v>-1</v>
@@ -4287,24 +4289,24 @@
         <v>2</v>
       </c>
       <c r="B65" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="C65" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="D65" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="E65" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
+      </c>
+      <c r="F65" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-6</v>
-      </c>
-      <c r="F65" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
       </c>
       <c r="G65" s="9" t="n">
         <v>-1</v>
@@ -4351,24 +4353,24 @@
         <v>3</v>
       </c>
       <c r="B66" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="C66" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>10</v>
+      </c>
+      <c r="D66" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
+      </c>
+      <c r="E66" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>15</v>
       </c>
-      <c r="D66" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
-      </c>
-      <c r="E66" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
-      </c>
       <c r="F66" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>0</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="G66" s="9" t="n">
         <v>-1</v>
@@ -4415,24 +4417,24 @@
         <v>4</v>
       </c>
       <c r="B67" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="C67" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="D67" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="E67" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="F67" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="G67" s="9" t="n">
         <v>-1</v>
@@ -4479,24 +4481,24 @@
         <v>5</v>
       </c>
       <c r="B68" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
+      </c>
+      <c r="C68" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
+      </c>
+      <c r="D68" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
+      </c>
+      <c r="E68" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
+      </c>
+      <c r="F68" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>0</v>
-      </c>
-      <c r="C68" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
-      </c>
-      <c r="D68" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
-      </c>
-      <c r="E68" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
-      </c>
-      <c r="F68" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
       </c>
       <c r="G68" s="9" t="n">
         <v>-1</v>
@@ -4566,24 +4568,24 @@
         <v>1</v>
       </c>
       <c r="B70" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
+      </c>
+      <c r="C70" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
+      </c>
+      <c r="D70" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>9</v>
+      </c>
+      <c r="E70" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>19</v>
       </c>
-      <c r="C70" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
-      </c>
-      <c r="D70" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
-      </c>
-      <c r="E70" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
-      </c>
       <c r="F70" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="G70" s="9" t="n">
         <v>-1</v>
@@ -4630,24 +4632,24 @@
         <v>2</v>
       </c>
       <c r="B71" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="C71" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D71" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E71" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="F71" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>20</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G71" s="9" t="n">
         <v>-1</v>
@@ -4694,24 +4696,24 @@
         <v>3</v>
       </c>
       <c r="B72" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="C72" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>13</v>
       </c>
       <c r="D72" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="E72" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="F72" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="G72" s="9" t="n">
         <v>-1</v>
@@ -4758,24 +4760,24 @@
         <v>4</v>
       </c>
       <c r="B73" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="C73" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="D73" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E73" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="F73" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="G73" s="9" t="n">
         <v>-1</v>
@@ -4822,24 +4824,24 @@
         <v>5</v>
       </c>
       <c r="B74" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="C74" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D74" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
+      </c>
+      <c r="E74" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
+      </c>
+      <c r="F74" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>6</v>
-      </c>
-      <c r="E74" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
-      </c>
-      <c r="F74" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
       </c>
       <c r="G74" s="9" t="n">
         <v>-1</v>
@@ -4909,24 +4911,24 @@
         <v>1</v>
       </c>
       <c r="B76" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="C76" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D76" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="E76" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="F76" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="G76" s="9" t="n">
         <v>-1</v>
@@ -4973,24 +4975,24 @@
         <v>2</v>
       </c>
       <c r="B77" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
+      </c>
+      <c r="C77" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
+      </c>
+      <c r="D77" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
+      </c>
+      <c r="E77" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>0</v>
+      </c>
+      <c r="F77" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-10</v>
-      </c>
-      <c r="C77" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
-      </c>
-      <c r="D77" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
-      </c>
-      <c r="E77" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
-      </c>
-      <c r="F77" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
       </c>
       <c r="G77" s="9" t="n">
         <v>-1</v>
@@ -5037,24 +5039,24 @@
         <v>3</v>
       </c>
       <c r="B78" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="C78" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="D78" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="E78" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="F78" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>20</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="G78" s="9" t="n">
         <v>-1</v>
@@ -5101,24 +5103,24 @@
         <v>4</v>
       </c>
       <c r="B79" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C79" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="D79" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="E79" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="F79" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="G79" s="9" t="n">
         <v>-1</v>
@@ -5165,24 +5167,24 @@
         <v>5</v>
       </c>
       <c r="B80" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="C80" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="D80" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E80" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="F80" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="G80" s="9" t="n">
         <v>-1</v>
@@ -5252,24 +5254,24 @@
         <v>1</v>
       </c>
       <c r="B82" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
+      </c>
+      <c r="C82" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
+      </c>
+      <c r="D82" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
+      </c>
+      <c r="E82" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
+      </c>
+      <c r="F82" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-9</v>
-      </c>
-      <c r="C82" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
-      </c>
-      <c r="D82" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
-      </c>
-      <c r="E82" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
-      </c>
-      <c r="F82" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
       </c>
       <c r="G82" s="9" t="n">
         <v>-1</v>
@@ -5316,24 +5318,24 @@
         <v>2</v>
       </c>
       <c r="B83" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="C83" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
+      </c>
+      <c r="D83" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
+      </c>
+      <c r="E83" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
+      </c>
+      <c r="F83" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>8</v>
-      </c>
-      <c r="D83" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
-      </c>
-      <c r="E83" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
-      </c>
-      <c r="F83" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
       </c>
       <c r="G83" s="9" t="n">
         <v>-1</v>
@@ -5380,24 +5382,24 @@
         <v>3</v>
       </c>
       <c r="B84" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="C84" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D84" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="E84" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="F84" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="G84" s="9" t="n">
         <v>-1</v>
@@ -5444,24 +5446,24 @@
         <v>4</v>
       </c>
       <c r="B85" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="C85" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D85" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="E85" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="F85" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>20</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="G85" s="9" t="n">
         <v>-1</v>
@@ -5508,24 +5510,24 @@
         <v>5</v>
       </c>
       <c r="B86" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C86" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="D86" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="E86" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="F86" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="G86" s="9" t="n">
         <v>-1</v>
@@ -5595,24 +5597,24 @@
         <v>1</v>
       </c>
       <c r="B88" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="C88" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="D88" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="E88" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="F88" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="G88" s="9" t="n">
         <v>-1</v>
@@ -5659,24 +5661,24 @@
         <v>2</v>
       </c>
       <c r="B89" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="C89" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D89" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="E89" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="F89" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G89" s="9" t="n">
         <v>-1</v>
@@ -5723,24 +5725,24 @@
         <v>3</v>
       </c>
       <c r="B90" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="C90" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="D90" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="E90" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="F90" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="G90" s="9" t="n">
         <v>-1</v>
@@ -5787,24 +5789,24 @@
         <v>4</v>
       </c>
       <c r="B91" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="C91" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>20</v>
       </c>
       <c r="D91" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
+      </c>
+      <c r="E91" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>8</v>
       </c>
-      <c r="E91" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+      <c r="F91" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>19</v>
-      </c>
-      <c r="F91" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
       </c>
       <c r="G91" s="9" t="n">
         <v>-1</v>
@@ -5851,24 +5853,24 @@
         <v>5</v>
       </c>
       <c r="B92" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="C92" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>7</v>
       </c>
       <c r="D92" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>0</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="E92" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="F92" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="G92" s="9" t="n">
         <v>-1</v>
@@ -5938,24 +5940,24 @@
         <v>1</v>
       </c>
       <c r="B94" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="C94" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="D94" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="E94" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="F94" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="G94" s="9" t="n">
         <v>-1</v>
@@ -6002,24 +6004,24 @@
         <v>2</v>
       </c>
       <c r="B95" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>20</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="C95" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="D95" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="E95" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F95" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="G95" s="9" t="n">
         <v>-1</v>
@@ -6066,24 +6068,24 @@
         <v>3</v>
       </c>
       <c r="B96" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="C96" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="D96" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>0</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="E96" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="F96" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="G96" s="9" t="n">
         <v>-1</v>
@@ -6130,24 +6132,24 @@
         <v>4</v>
       </c>
       <c r="B97" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="C97" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>0</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-8</v>
       </c>
       <c r="D97" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="E97" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="F97" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="G97" s="9" t="n">
         <v>-1</v>
@@ -6194,24 +6196,24 @@
         <v>5</v>
       </c>
       <c r="B98" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="C98" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D98" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
       </c>
       <c r="E98" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
       </c>
       <c r="F98" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="G98" s="9" t="n">
         <v>-1</v>
@@ -6281,24 +6283,24 @@
         <v>1</v>
       </c>
       <c r="B100" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="C100" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
+      </c>
+      <c r="D100" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
+      </c>
+      <c r="E100" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
+      </c>
+      <c r="F100" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>18</v>
-      </c>
-      <c r="D100" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
-      </c>
-      <c r="E100" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
-      </c>
-      <c r="F100" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
       </c>
       <c r="G100" s="9" t="n">
         <v>-1</v>
@@ -6345,24 +6347,24 @@
         <v>2</v>
       </c>
       <c r="B101" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="C101" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
+      </c>
+      <c r="D101" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>25</v>
       </c>
-      <c r="D101" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
-      </c>
       <c r="E101" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="F101" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>0</v>
       </c>
       <c r="G101" s="9" t="n">
         <v>-1</v>
@@ -6409,24 +6411,24 @@
         <v>3</v>
       </c>
       <c r="B102" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="C102" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="D102" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="E102" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="F102" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="G102" s="9" t="n">
         <v>-1</v>
@@ -6473,24 +6475,24 @@
         <v>4</v>
       </c>
       <c r="B103" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="C103" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="D103" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="E103" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>21</v>
       </c>
       <c r="F103" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="G103" s="9" t="n">
         <v>-1</v>
@@ -6537,24 +6539,24 @@
         <v>5</v>
       </c>
       <c r="B104" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
+      </c>
+      <c r="C104" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
+      </c>
+      <c r="D104" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
+      </c>
+      <c r="E104" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
+      </c>
+      <c r="F104" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>0</v>
-      </c>
-      <c r="C104" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
-      </c>
-      <c r="D104" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
-      </c>
-      <c r="E104" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
-      </c>
-      <c r="F104" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
       </c>
       <c r="G104" s="9" t="n">
         <v>-1</v>
@@ -6624,24 +6626,24 @@
         <v>1</v>
       </c>
       <c r="B106" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>24</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="C106" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D106" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>18</v>
       </c>
       <c r="E106" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="F106" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="G106" s="9" t="n">
         <v>-1</v>
@@ -6688,24 +6690,24 @@
         <v>2</v>
       </c>
       <c r="B107" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="C107" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="D107" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
       </c>
       <c r="E107" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="F107" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>2</v>
       </c>
       <c r="G107" s="9" t="n">
         <v>-1</v>
@@ -6752,24 +6754,24 @@
         <v>3</v>
       </c>
       <c r="B108" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="C108" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="D108" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
+      </c>
+      <c r="E108" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
+      </c>
+      <c r="F108" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>5</v>
-      </c>
-      <c r="E108" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
-      </c>
-      <c r="F108" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
       </c>
       <c r="G108" s="9" t="n">
         <v>-1</v>
@@ -6816,24 +6818,24 @@
         <v>4</v>
       </c>
       <c r="B109" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C109" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>25</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="D109" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="E109" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="F109" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="G109" s="9" t="n">
         <v>-1</v>
@@ -6880,24 +6882,24 @@
         <v>5</v>
       </c>
       <c r="B110" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="C110" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="D110" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>0</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="E110" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
       </c>
       <c r="F110" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>6</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="G110" s="9" t="n">
         <v>-1</v>
@@ -6967,24 +6969,24 @@
         <v>1</v>
       </c>
       <c r="B112" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="C112" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>20</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="D112" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="E112" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="F112" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="G112" s="9" t="n">
         <v>-1</v>
@@ -7031,24 +7033,24 @@
         <v>2</v>
       </c>
       <c r="B113" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="C113" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>14</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="D113" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="E113" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
       </c>
       <c r="F113" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="G113" s="9" t="n">
         <v>-1</v>
@@ -7095,24 +7097,24 @@
         <v>3</v>
       </c>
       <c r="B114" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="C114" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="D114" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>15</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="E114" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
+      </c>
+      <c r="F114" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>20</v>
-      </c>
-      <c r="F114" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
       </c>
       <c r="G114" s="9" t="n">
         <v>-1</v>
@@ -7159,24 +7161,24 @@
         <v>4</v>
       </c>
       <c r="B115" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>25</v>
       </c>
       <c r="C115" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D115" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="E115" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>19</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="F115" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="G115" s="9" t="n">
         <v>-1</v>
@@ -7223,24 +7225,24 @@
         <v>5</v>
       </c>
       <c r="B116" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="C116" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-9</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>10</v>
       </c>
       <c r="D116" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="E116" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>13</v>
       </c>
       <c r="F116" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>8</v>
       </c>
       <c r="G116" s="9" t="n">
         <v>-1</v>
@@ -7310,24 +7312,24 @@
         <v>1</v>
       </c>
       <c r="B118" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>15</v>
       </c>
       <c r="C118" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>1</v>
       </c>
       <c r="D118" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="E118" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="F118" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-3</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="G118" s="9" t="n">
         <v>-1</v>
@@ -7374,24 +7376,24 @@
         <v>2</v>
       </c>
       <c r="B119" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="C119" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="D119" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="E119" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="F119" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-2</v>
       </c>
       <c r="G119" s="9" t="n">
         <v>-1</v>
@@ -7438,24 +7440,24 @@
         <v>3</v>
       </c>
       <c r="B120" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>12</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-3</v>
       </c>
       <c r="C120" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-6</v>
       </c>
       <c r="D120" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>4</v>
       </c>
       <c r="E120" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>-1</v>
       </c>
       <c r="F120" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="G120" s="9" t="n">
         <v>-1</v>
@@ -7502,24 +7504,24 @@
         <v>4</v>
       </c>
       <c r="B121" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>9</v>
       </c>
       <c r="C121" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>7</v>
       </c>
       <c r="D121" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
       </c>
       <c r="E121" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
       </c>
       <c r="F121" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>11</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="G121" s="9" t="n">
         <v>-1</v>
@@ -7566,24 +7568,24 @@
         <v>5</v>
       </c>
       <c r="B122" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>5</v>
+      </c>
+      <c r="C122" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
+      </c>
+      <c r="D122" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>20</v>
+      </c>
+      <c r="E122" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>24</v>
+      </c>
+      <c r="F122" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>1</v>
-      </c>
-      <c r="C122" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-6</v>
-      </c>
-      <c r="D122" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-4</v>
-      </c>
-      <c r="E122" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-9</v>
-      </c>
-      <c r="F122" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-10</v>
       </c>
       <c r="G122" s="9" t="n">
         <v>-1</v>
@@ -7653,24 +7655,24 @@
         <v>1</v>
       </c>
       <c r="B124" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-5</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>14</v>
       </c>
       <c r="C124" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="D124" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>12</v>
       </c>
       <c r="E124" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>10</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="F124" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="G124" s="9" t="n">
         <v>-1</v>
@@ -7717,24 +7719,24 @@
         <v>2</v>
       </c>
       <c r="B125" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
       </c>
       <c r="C125" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="D125" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>13</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="E125" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>16</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>6</v>
       </c>
       <c r="F125" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-10</v>
       </c>
       <c r="G125" s="9" t="n">
         <v>-1</v>
@@ -7781,24 +7783,24 @@
         <v>3</v>
       </c>
       <c r="B126" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>16</v>
+      </c>
+      <c r="C126" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
+      </c>
+      <c r="D126" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>14</v>
       </c>
-      <c r="C126" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
-      </c>
-      <c r="D126" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>17</v>
-      </c>
       <c r="E126" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-4</v>
       </c>
       <c r="F126" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>-7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>22</v>
       </c>
       <c r="G126" s="9" t="n">
         <v>-1</v>
@@ -7845,24 +7847,24 @@
         <v>4</v>
       </c>
       <c r="B127" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>7</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>23</v>
       </c>
       <c r="C127" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>17</v>
+      </c>
+      <c r="D127" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>3</v>
+      </c>
+      <c r="E127" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-5</v>
+      </c>
+      <c r="F127" s="9" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
         <v>2</v>
-      </c>
-      <c r="D127" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>18</v>
-      </c>
-      <c r="E127" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>2</v>
-      </c>
-      <c r="F127" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>8</v>
       </c>
       <c r="G127" s="9" t="n">
         <v>-1</v>
@@ -7909,24 +7911,24 @@
         <v>5</v>
       </c>
       <c r="B128" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>1</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-9</v>
       </c>
       <c r="C128" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>4</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-1</v>
       </c>
       <c r="D128" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>21</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>11</v>
       </c>
       <c r="E128" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>23</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>-7</v>
       </c>
       <c r="F128" s="9" t="n">
-        <f aca="false">RANDBETWEEN(-10,25)</f>
-        <v>22</v>
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(-10,25)</f>
+        <v>19</v>
       </c>
       <c r="G128" s="9" t="n">
         <v>-1</v>

</xml_diff>